<commit_message>
final sub for pub
</commit_message>
<xml_diff>
--- a/paper/Submissions/PlantCell/TPC accepted sub/Supplemental Figures and Tables/SDS 1. Mean of B. cinerea Lesion Size.xlsx
+++ b/paper/Submissions/PlantCell/TPC accepted sub/Supplemental Figures and Tables/SDS 1. Mean of B. cinerea Lesion Size.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesol\Documents\Projects\BcSolGWAS\paper\Submissions\PlantCell\TPC revision\Final\Supplemental Figures and Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nesol\Documents\Projects\BcSolGWAS\paper\Submissions\PlantCell\TPC accepted sub\Supplemental Figures and Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49F9C7C-BE86-4957-9CA3-78DA8CEC52A7}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59441D42-D4D2-4ACC-A3FB-254F4099FE9C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10920" windowHeight="7060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10920" windowHeight="7056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDS1" sheetId="1" r:id="rId1"/>
@@ -4370,16 +4370,17 @@
   <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.453125" style="8" customWidth="1"/>
-    <col min="2" max="15" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.44140625" style="8" customWidth="1"/>
+    <col min="2" max="15" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="22.8" x14ac:dyDescent="0.3">
       <c r="A1" s="6"/>
       <c r="B1" s="1" t="s">
         <v>1142</v>
@@ -4398,7 +4399,7 @@
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="3" t="s">
         <v>96</v>
@@ -4419,7 +4420,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="4" t="s">
         <v>106</v>
@@ -4464,7 +4465,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -4511,7 +4512,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>1</v>
       </c>
@@ -4558,7 +4559,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>2</v>
       </c>
@@ -4605,7 +4606,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -4652,7 +4653,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -4699,7 +4700,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -4746,7 +4747,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -4793,7 +4794,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>7</v>
       </c>
@@ -4840,7 +4841,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -4887,7 +4888,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -4934,7 +4935,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="15" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>11</v>
       </c>
@@ -5028,7 +5029,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
@@ -5122,7 +5123,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
         <v>14</v>
       </c>
@@ -5169,7 +5170,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>15</v>
       </c>
@@ -5216,7 +5217,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>16</v>
       </c>
@@ -5263,7 +5264,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
         <v>17</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
@@ -5357,7 +5358,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>19</v>
       </c>
@@ -5404,7 +5405,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
@@ -5451,7 +5452,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
@@ -5498,7 +5499,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>22</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
@@ -5592,7 +5593,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>24</v>
       </c>
@@ -5639,7 +5640,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="29" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>25</v>
       </c>
@@ -5686,7 +5687,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="30" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>26</v>
       </c>
@@ -5733,7 +5734,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="31" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>27</v>
       </c>
@@ -5780,7 +5781,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="32" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>28</v>
       </c>
@@ -5827,7 +5828,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>29</v>
       </c>
@@ -5874,7 +5875,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>30</v>
       </c>
@@ -5921,7 +5922,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>31</v>
       </c>
@@ -5968,7 +5969,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>32</v>
       </c>
@@ -6015,7 +6016,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>33</v>
       </c>
@@ -6062,7 +6063,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>34</v>
       </c>
@@ -6109,7 +6110,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>35</v>
       </c>
@@ -6156,7 +6157,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>36</v>
       </c>
@@ -6203,7 +6204,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>37</v>
       </c>
@@ -6250,7 +6251,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="42" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
         <v>38</v>
       </c>
@@ -6297,7 +6298,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="43" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A43" s="7" t="s">
         <v>39</v>
       </c>
@@ -6344,7 +6345,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="44" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A44" s="7" t="s">
         <v>40</v>
       </c>
@@ -6391,7 +6392,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="45" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A45" s="7" t="s">
         <v>41</v>
       </c>
@@ -6438,7 +6439,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A46" s="7" t="s">
         <v>42</v>
       </c>
@@ -6485,7 +6486,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="47" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>43</v>
       </c>
@@ -6532,7 +6533,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="48" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>44</v>
       </c>
@@ -6579,7 +6580,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="49" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>45</v>
       </c>
@@ -6626,7 +6627,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="50" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A50" s="7" t="s">
         <v>46</v>
       </c>
@@ -6673,7 +6674,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A51" s="7" t="s">
         <v>47</v>
       </c>
@@ -6720,7 +6721,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="52" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>48</v>
       </c>
@@ -6767,7 +6768,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="53" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A53" s="7" t="s">
         <v>49</v>
       </c>
@@ -6814,7 +6815,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>50</v>
       </c>
@@ -6861,7 +6862,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="55" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A55" s="7" t="s">
         <v>51</v>
       </c>
@@ -6908,7 +6909,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="56" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>52</v>
       </c>
@@ -6955,7 +6956,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="57" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>53</v>
       </c>
@@ -7002,7 +7003,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>54</v>
       </c>
@@ -7049,7 +7050,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="59" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A59" s="7" t="s">
         <v>55</v>
       </c>
@@ -7096,7 +7097,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="60" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A60" s="9">
         <v>2004</v>
       </c>
@@ -7143,7 +7144,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="61" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A61" s="9">
         <v>94.4</v>
       </c>
@@ -7190,7 +7191,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="62" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>56</v>
       </c>
@@ -7237,7 +7238,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>57</v>
       </c>
@@ -7284,7 +7285,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="64" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A64" s="7" t="s">
         <v>58</v>
       </c>
@@ -7331,7 +7332,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="65" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A65" s="7" t="s">
         <v>59</v>
       </c>
@@ -7378,7 +7379,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="66" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A66" s="7" t="s">
         <v>60</v>
       </c>
@@ -7425,7 +7426,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A67" s="7" t="s">
         <v>61</v>
       </c>
@@ -7472,7 +7473,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="68" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A68" s="7" t="s">
         <v>62</v>
       </c>
@@ -7519,7 +7520,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="69" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A69" s="7" t="s">
         <v>63</v>
       </c>
@@ -7566,7 +7567,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="70" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A70" s="7" t="s">
         <v>64</v>
       </c>
@@ -7613,7 +7614,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="71" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A71" s="7" t="s">
         <v>65</v>
       </c>
@@ -7660,7 +7661,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>66</v>
       </c>
@@ -7707,7 +7708,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="73" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
         <v>67</v>
       </c>
@@ -7754,7 +7755,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="74" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
         <v>68</v>
       </c>
@@ -7801,7 +7802,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="75" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A75" s="7" t="s">
         <v>69</v>
       </c>
@@ -7848,7 +7849,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A76" s="7" t="s">
         <v>70</v>
       </c>
@@ -7895,7 +7896,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A77" s="7" t="s">
         <v>71</v>
       </c>
@@ -7942,7 +7943,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="78" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A78" s="7" t="s">
         <v>72</v>
       </c>
@@ -7989,7 +7990,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="79" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
         <v>73</v>
       </c>
@@ -8036,7 +8037,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="80" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A80" s="7" t="s">
         <v>74</v>
       </c>
@@ -8083,7 +8084,7 @@
         <v>1051</v>
       </c>
     </row>
-    <row r="81" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>75</v>
       </c>
@@ -8130,7 +8131,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A82" s="7" t="s">
         <v>76</v>
       </c>
@@ -8177,7 +8178,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="83" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A83" s="7" t="s">
         <v>77</v>
       </c>
@@ -8224,7 +8225,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="84" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A84" s="7" t="s">
         <v>78</v>
       </c>
@@ -8271,7 +8272,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="85" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A85" s="7" t="s">
         <v>79</v>
       </c>
@@ -8318,7 +8319,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="86" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A86" s="7" t="s">
         <v>80</v>
       </c>
@@ -8365,7 +8366,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A87" s="7" t="s">
         <v>81</v>
       </c>
@@ -8412,7 +8413,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="88" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
         <v>82</v>
       </c>
@@ -8459,7 +8460,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="89" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A89" s="7" t="s">
         <v>83</v>
       </c>
@@ -8506,7 +8507,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="90" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
         <v>84</v>
       </c>
@@ -8553,7 +8554,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="91" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A91" s="7" t="s">
         <v>85</v>
       </c>
@@ -8600,7 +8601,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A92" s="7" t="s">
         <v>86</v>
       </c>
@@ -8647,7 +8648,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A93" s="7" t="s">
         <v>87</v>
       </c>
@@ -8694,7 +8695,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="94" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A94" s="7" t="s">
         <v>88</v>
       </c>
@@ -8741,7 +8742,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="95" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>89</v>
       </c>
@@ -8788,7 +8789,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="96" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>90</v>
       </c>
@@ -8835,7 +8836,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="97" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A97" s="7" t="s">
         <v>91</v>
       </c>
@@ -8882,7 +8883,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A98" s="7" t="s">
         <v>92</v>
       </c>
@@ -8929,7 +8930,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="99" spans="1:15" ht="20" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:15" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A99" s="7" t="s">
         <v>1126</v>
       </c>

</xml_diff>